<commit_message>
Dodaj powiązania ryzyk do celów projektu
</commit_message>
<xml_diff>
--- a/Cwiczenie-4/Ryzyka.xlsx
+++ b/Cwiczenie-4/Ryzyka.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzyka" sheetId="1" r:id="rId1"/>
     <sheet name="Mitygacja" sheetId="4" r:id="rId2"/>
-    <sheet name="Zliczenie ryzyk" sheetId="6" r:id="rId3"/>
-    <sheet name="Dystrybucja ryzyk" sheetId="8" r:id="rId4"/>
+    <sheet name="Powiązanie z celami" sheetId="9" r:id="rId3"/>
+    <sheet name="Zliczenie ryzyk" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mitygacja!$A$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Powiązanie z celami'!$A$2:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ryzyka!$A$1:$G$19</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
   <si>
     <t>Zmniejszenie wpływu</t>
   </si>
@@ -211,9 +212,6 @@
     <t>Wpływ</t>
   </si>
   <si>
-    <t>Zaangażowanie współpracowników ze strony partnera</t>
-  </si>
-  <si>
     <t>Jakość danych od partnerów</t>
   </si>
   <si>
@@ -241,15 +239,9 @@
     <t>Brak współpracy użytkowników w trakcie projektu</t>
   </si>
   <si>
-    <t>Analiza wymagań użytkowników. Możliwe niezgodności dotyczące wymagań stawianych aplikacji.</t>
-  </si>
-  <si>
     <t>Beta testy aplikacji mobilnej i zastosowanie się do sugestii testerów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Partnerzy nie przesyłają danych o wydarzeniach z odpowiednią częstotliwością lub przesłane dane są niekompletne. Wpływa to znacząco na użyteczność aplikacji. </t>
-  </si>
-  <si>
     <t>Zewnętrznych zależności</t>
   </si>
   <si>
@@ -332,13 +324,59 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Nawiązanie współpracy z organizatorami</t>
+  </si>
+  <si>
+    <t>Uzyskanie stałej bazy użytkowników</t>
+  </si>
+  <si>
+    <t>Serwer obsługi zapytań</t>
+  </si>
+  <si>
+    <t>Zwiększenie efektywności akcji reklamowych</t>
+  </si>
+  <si>
+    <t>Aplikacja mobilna</t>
+  </si>
+  <si>
+    <t>API udostępniane organizatorom</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cele projektu </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concerto</t>
+    </r>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Zaangażowanie współpracujących organizatorów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procesy biznesowe zarządzania informacjami o wydarzeniach zaprojektowane nieadekwatnie do wymagań współpracujących organizatorów. Wpływa to znacząco na użyteczność aplikacji mobilnej. </t>
+  </si>
+  <si>
+    <t>Nie zrozumienie funkcjonalności aplikacji mobilnej. Niska intucyjność obsługi, niska ocena wyglądu aplikacji. Błędna analiza wymagań użytkowników aplikacji.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +439,14 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -410,7 +456,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -456,6 +502,24 @@
         <color theme="6"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -513,7 +577,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -577,6 +641,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -700,827 +785,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="121"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="21"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Dystrybucja ryzyk</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.4860870844390168E-2"/>
-          <c:y val="0.10244076183253724"/>
-          <c:w val="0.8896734009737044"/>
-          <c:h val="0.78494408252847148"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FFC000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FFC000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="15"/>
-            <c:marker>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FFC000"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$2</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ORGZ1</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$3</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ORGZ2</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$4</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>PLAN1</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$5</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>PLAN2</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$6</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>PLAN3</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$7</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>PLAN4</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$8</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>TECH1</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$9</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>TECH2</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$10</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>TECH3</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.9604102361207746E-2"/>
-                  <c:y val="-6.1935460125098554E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$11</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>TECH4</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$12</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZAOP1</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="11"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.9604102361207746E-2"/>
-                  <c:y val="-6.1935460125098554E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$13</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZAOP2</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="12"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.7258426349172173E-2"/>
-                  <c:y val="-6.1935460125098554E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$14</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZAOP3</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="13"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.7258426349172173E-2"/>
-                  <c:y val="-6.1935460125098554E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$15</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZAOP4</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="14"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$16</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZEWN1</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="15"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$17</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZEWN2</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="16"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.9604102361207746E-2"/>
-                  <c:y val="-6.1935460125098554E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$18</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZEWN4</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="17"/>
-              <c:layout/>
-              <c:tx>
-                <c:strRef>
-                  <c:f>Ryzyka!$A$19</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>ZEWN5</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
-              </c:tx>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Ryzyka!$E$2:$E$19</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Ryzyka!$F$2:$F$19</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="132662784"/>
-        <c:axId val="132664704"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="132662784"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="16"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Praw</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>dopodobieństwo</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="in"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132664704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="0.4"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="132664704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="5"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pl-PL"/>
-                  <a:t>Koszt</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132662784"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-        <c:minorUnit val="0.2"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>761998</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12698</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1795,7 +1059,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba wystąpień" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba wystąpień" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -2291,26 +1555,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="8"/>
-    <col min="6" max="6" width="8.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8"/>
-    <col min="8" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="8"/>
+    <col min="6" max="6" width="8.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="8"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2333,18 +1597,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="56">
       <c r="A2" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="E2" s="10">
         <v>2</v>
@@ -2357,18 +1621,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="56">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -2381,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="84">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -2405,7 +1669,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="70">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -2429,7 +1693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="56">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -2453,7 +1717,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +1738,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="42">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -2498,7 +1762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -2522,7 +1786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="56">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -2546,7 +1810,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="56">
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
@@ -2570,7 +1834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -2581,7 +1845,7 @@
         <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E12" s="8">
         <v>2</v>
@@ -2594,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="42">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2618,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -2642,7 +1906,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -2663,18 +1927,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="84">
       <c r="A16" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E16" s="8">
         <v>16</v>
@@ -2687,18 +1951,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="56">
       <c r="A17" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E17" s="8">
         <v>8</v>
@@ -2711,18 +1975,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="70">
       <c r="A18" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E18" s="8">
         <v>4</v>
@@ -2735,18 +1999,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="56">
       <c r="A19" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="8">
         <v>16</v>
@@ -2782,7 +2046,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2795,28 +2059,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -2825,9 +2089,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28">
       <c r="A2" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="str">
         <f>VLOOKUP(A2, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -2837,22 +2101,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="str">
         <f>VLOOKUP(A3, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
-        <v>Zaangażowanie współpracowników ze strony partnera</v>
+        <v>Zaangażowanie współpracujących organizatorów</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="42">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -2867,7 +2131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -2879,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -2897,7 +2161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -2909,7 +2173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -2924,7 +2188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -2939,7 +2203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="42">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -2951,10 +2215,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -2969,7 +2233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="42">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -2984,7 +2248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -2999,7 +2263,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -3014,7 +2278,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="42">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -3029,7 +2293,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -3041,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="42">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
@@ -3056,10 +2320,10 @@
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="42">
       <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
@@ -3071,10 +2335,10 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28">
       <c r="A19" s="12" t="s">
         <v>56</v>
       </c>
@@ -3089,7 +2353,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
@@ -3104,7 +2368,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28">
       <c r="A21" s="12" t="s">
         <v>56</v>
       </c>
@@ -3116,10 +2380,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="42">
       <c r="A22" s="12" t="s">
         <v>56</v>
       </c>
@@ -3131,12 +2395,12 @@
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="42">
       <c r="A23" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B23" s="3" t="str">
         <f>VLOOKUP(A23, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3146,12 +2410,12 @@
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="70">
       <c r="A24" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B24" s="3" t="str">
         <f>VLOOKUP(A24, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3161,12 +2425,12 @@
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28">
       <c r="A25" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="str">
         <f>VLOOKUP(A25, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3176,12 +2440,12 @@
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="56">
       <c r="A26" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" s="3" t="str">
         <f>VLOOKUP(A26, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3191,12 +2455,12 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28">
       <c r="A27" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="str">
         <f>VLOOKUP(A27, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3206,27 +2470,27 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" s="3" t="str">
         <f>VLOOKUP(A28, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Konkurencja</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" ht="42">
       <c r="A29" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B29" s="3" t="str">
         <f>VLOOKUP(A29, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
@@ -3236,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3257,156 +2521,363 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="8" width="20.83203125" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="1" spans="1:8" s="22" customFormat="1" ht="28" customHeight="1">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" s="23" customFormat="1" ht="28" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="20">
-        <v>1</v>
-      </c>
-      <c r="C4" s="20">
-        <v>2</v>
-      </c>
-      <c r="D4" s="20">
-        <v>3</v>
-      </c>
-      <c r="E4" s="20">
-        <v>4</v>
-      </c>
-      <c r="F4" s="20">
-        <v>5</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
-        <v>1</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
-        <v>2</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
-        <v>4</v>
-      </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
-        <v>8</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-      <c r="C10" s="18">
-        <v>1</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>100</v>
+    </row>
+    <row r="3" spans="1:8" ht="28">
+      <c r="A3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f>VLOOKUP(A3, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Brak współpracy użytkowników w trakcie projektu</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="42">
+      <c r="A4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f>VLOOKUP(A4, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Zaangażowanie współpracujących organizatorów</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42">
+      <c r="A5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>VLOOKUP(A5, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Niewystarczające kwalifikacje i doświadczenie członków zespołu</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>VLOOKUP(A6, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Krytyczne uwarunkowania czasowe</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>VLOOKUP(A7, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Gęstość pracochłonności</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28">
+      <c r="A8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>VLOOKUP(A8, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Brak doświadczenia kierownika projektu</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28">
+      <c r="A9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>VLOOKUP(A9, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Dynamiczność rynku technologii mobilnych</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28">
+      <c r="A10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>VLOOKUP(A10, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Jednoznaczność specyfikacji funkcjonalnej</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>VLOOKUP(A11, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Złożoność systemu</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>VLOOKUP(A12, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Sprawność operacyjna</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>VLOOKUP(A13, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Elastyczność kosztów</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>VLOOKUP(A14, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Elastyczność zakresu projektu</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>VLOOKUP(A15, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Poparcie biznesowe inwestorów</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f>VLOOKUP(A16, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Przyjęcie aplikacji mobilnej przez użytkowników</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>VLOOKUP(A17, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Zbyt mała liczba współpracujących organizatorów</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f>VLOOKUP(A18, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Jakość danych od partnerów</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>VLOOKUP(A19, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Usługi serwerowe</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f>VLOOKUP(A20, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
+        <v>Konkurencja</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <autoFilter ref="A2:B20">
+    <sortState ref="A2:E29">
+      <sortCondition ref="A1:A29"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="2">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3418,15 +2889,157 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14">
+      <c r="A1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14">
+      <c r="A3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="A4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>2</v>
+      </c>
+      <c r="D4" s="20">
+        <v>3</v>
+      </c>
+      <c r="E4" s="20">
+        <v>4</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14">
+      <c r="A5" s="20">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="14">
+      <c r="A6" s="20">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="14">
+      <c r="A7" s="20">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14">
+      <c r="A8" s="20">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" thickBot="1">
+      <c r="A9" s="20">
+        <v>16</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" thickTop="1">
+      <c r="A10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18">
+        <v>1</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" ht="15" customHeight="1">
+      <c r="C18" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Popraw tablice zbiorcze w kompilacji ryzyk
</commit_message>
<xml_diff>
--- a/Cwiczenie-4/Ryzyka.xlsx
+++ b/Cwiczenie-4/Ryzyka.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
-  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="16440" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzyka" sheetId="1" r:id="rId1"/>
     <sheet name="Mitygacja" sheetId="4" r:id="rId2"/>
     <sheet name="Powiązanie z celami" sheetId="9" r:id="rId3"/>
-    <sheet name="Zliczenie ryzyk" sheetId="6" r:id="rId4"/>
+    <sheet name="Zliczenie ryzyk" sheetId="17" r:id="rId4"/>
+    <sheet name="Zliczenie ryzyk szczegółowe" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mitygacja!$A$1:$D$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Powiązanie z celami'!$A$2:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ryzyka!$A$1:$G$19</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="26" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="118">
   <si>
     <t>Zmniejszenie wpływu</t>
   </si>
@@ -318,12 +319,6 @@
   </si>
   <si>
     <t>Liczba wystąpień</t>
-  </si>
-  <si>
-    <t>Zliczenie ryzyk</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>Nawiązanie współpracy z organizatorami</t>
@@ -370,6 +365,42 @@
   </si>
   <si>
     <t>Nie zrozumienie funkcjonalności aplikacji mobilnej. Niska intucyjność obsługi, niska ocena wyglądu aplikacji. Błędna analiza wymagań użytkowników aplikacji.</t>
+  </si>
+  <si>
+    <t>Zliczenie ryzyk według kosztów dla kategorii</t>
+  </si>
+  <si>
+    <t>Organizacyjne - Suma</t>
+  </si>
+  <si>
+    <t>Planowanie - Suma</t>
+  </si>
+  <si>
+    <t>Techniczne - Suma</t>
+  </si>
+  <si>
+    <t>Założeń opłacalności - Suma</t>
+  </si>
+  <si>
+    <t>Zewnętrznych zależności - Suma</t>
+  </si>
+  <si>
+    <t>Zliczenie ryzyk według wpływu</t>
+  </si>
+  <si>
+    <t>Liczba ryzyk</t>
+  </si>
+  <si>
+    <t>Niski wpływ
+(0-19)</t>
+  </si>
+  <si>
+    <t>Średni wpływ
+(20-39)</t>
+  </si>
+  <si>
+    <t>Wysoki wpływ
+(&gt; 40)</t>
   </si>
 </sst>
 </file>
@@ -433,18 +464,18 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -456,7 +487,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -476,35 +507,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color theme="6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color theme="6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -520,6 +522,24 @@
       <bottom style="thin">
         <color theme="1" tint="0.249977111117893"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -577,7 +597,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -615,53 +635,84 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -718,67 +769,1196 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="318">
     <dxf>
       <border>
-        <top style="double">
-          <color theme="6"/>
-        </top>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <top style="double">
-          <color theme="6"/>
-        </top>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="double">
-          <color theme="6"/>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.59999389629810485"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.59999389629810485"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.59999389629810485"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF92D050"/>
         </left>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color rgb="FF92D050"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF92D050"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -788,7 +1968,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Tomasz Cudziło" refreshedDate="41260.08769803241" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="18">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Tomasz Cudziło" refreshedDate="41276.879710995374" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="18">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G19" sheet="Ryzyka"/>
   </cacheSource>
@@ -825,26 +2005,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Nazwa" numFmtId="0">
-      <sharedItems count="18">
-        <s v="Brak współpracy użytkowników w trakcie projektu"/>
-        <s v="Zaangażowanie współpracowników ze strony partnera"/>
-        <s v="Niewystarczające kwalifikacje i doświadczenie członków zespołu"/>
-        <s v="Krytyczne uwarunkowania czasowe"/>
-        <s v="Gęstość pracochłonności"/>
-        <s v="Brak doświadczenia kierownika projektu"/>
-        <s v="Dynamiczność rynku technologii mobilnych"/>
-        <s v="Jednoznaczność specyfikacji funkcjonalnej"/>
-        <s v="Złożoność systemu"/>
-        <s v="Sprawność operacyjna"/>
-        <s v="Elastyczność kosztów"/>
-        <s v="Elastyczność zakresu projektu"/>
-        <s v="Poparcie biznesowe inwestorów"/>
-        <s v="Przyjęcie aplikacji mobilnej przez użytkowników"/>
-        <s v="Zbyt mała liczba współpracujących organizatorów"/>
-        <s v="Jakość danych od partnerów"/>
-        <s v="Usługi serwerowe"/>
-        <s v="Konkurencja"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Opis" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -881,6 +2042,15 @@
         <n v="24"/>
         <n v="16"/>
       </sharedItems>
+      <fieldGroup base="6">
+        <rangePr autoStart="0" autoEnd="0" startNum="0" endNum="40" groupInterval="20"/>
+        <groupItems count="4">
+          <s v="&lt;0"/>
+          <s v="0-19"/>
+          <s v="20-40"/>
+          <s v="&gt;40"/>
+        </groupItems>
+      </fieldGroup>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -896,8 +2066,8 @@
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
-    <s v="Analiza wymagań użytkowników. Możliwe niezgodności dotyczące wymagań stawianych aplikacji."/>
+    <s v="Brak współpracy użytkowników w trakcie projektu"/>
+    <s v="Nie zrozumienie funkcjonalności aplikacji mobilnej. Niska intucyjność obsługi, niska ocena wyglądu aplikacji. Błędna analiza wymagań użytkowników aplikacji."/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
@@ -905,8 +2075,8 @@
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
-    <s v="Partnerzy nie przesyłają danych o wydarzeniach z odpowiednią częstotliwością lub przesłane dane są niekompletne. Wpływa to znacząco na użyteczność aplikacji. "/>
+    <s v="Zaangażowanie współpracujących organizatorów"/>
+    <s v="Procesy biznesowe zarządzania informacjami o wydarzeniach zaprojektowane nieadekwatnie do wymagań współpracujących organizatorów. Wpływa to znacząco na użyteczność aplikacji mobilnej. "/>
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
@@ -914,7 +2084,7 @@
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <s v="Niewystarczające kwalifikacje i doświadczenie członków zespołu"/>
     <s v="Projekt wymaga specjalistycznej wiedzy z zakresu przetwarzania obrazów. Zebranie zespołu posiadającego doświadczenie w tej dziedzinie jest nieopłacalne przy dostępnych zasobach projektu. Zespół po szkoleniu nadal może nie posiadać wystarczającej wiedzy."/>
     <x v="2"/>
     <x v="2"/>
@@ -923,7 +2093,7 @@
   <r>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <s v="Krytyczne uwarunkowania czasowe"/>
     <s v="Plan organizacji prac nad projektem nie pozwala na duże opóźnienia między zadaniami. Ścieżka krytyczna zawiera zdecydowaną większość zadań, opóźnienie jednego może wpłynąć znacznie na opóźnienie całego projektu."/>
     <x v="3"/>
     <x v="3"/>
@@ -932,7 +2102,7 @@
   <r>
     <x v="4"/>
     <x v="1"/>
-    <x v="4"/>
+    <s v="Gęstość pracochłonności"/>
     <s v="Plan organizacji projektu zakłada zarządzanie kilkoma zadaniami równolegle. W późniejszych etapach prac, manager może mieć problem z  nadzorem grupy zadań jednocześnie."/>
     <x v="4"/>
     <x v="2"/>
@@ -941,7 +2111,7 @@
   <r>
     <x v="5"/>
     <x v="1"/>
-    <x v="5"/>
+    <s v="Brak doświadczenia kierownika projektu"/>
     <m/>
     <x v="2"/>
     <x v="0"/>
@@ -950,7 +2120,7 @@
   <r>
     <x v="6"/>
     <x v="2"/>
-    <x v="6"/>
+    <s v="Dynamiczność rynku technologii mobilnych"/>
     <s v="Rynek technologii mobilnych jest podatny na zmiany. Wybrana platforma mobilna może się zdeaktualizować w bliskiej przyszłości. "/>
     <x v="3"/>
     <x v="0"/>
@@ -959,7 +2129,7 @@
   <r>
     <x v="7"/>
     <x v="2"/>
-    <x v="7"/>
+    <s v="Jednoznaczność specyfikacji funkcjonalnej"/>
     <s v="Niejasny opis funkcjonalności oferowanej organizatorom utrudnia nawiązanie współpracy. "/>
     <x v="3"/>
     <x v="1"/>
@@ -968,7 +2138,7 @@
   <r>
     <x v="8"/>
     <x v="2"/>
-    <x v="8"/>
+    <s v="Złożoność systemu"/>
     <s v="Projekt techniczny zakłada rozdzielenie na kilka niezależnych modułów, które muszą współpracować. Synchronizacja rozwoju modułów i weryfikacja ich współpracy jest nietrywialne."/>
     <x v="2"/>
     <x v="3"/>
@@ -977,7 +2147,7 @@
   <r>
     <x v="9"/>
     <x v="2"/>
-    <x v="9"/>
+    <s v="Sprawność operacyjna"/>
     <s v="Problemy z efektywną komunikacją między podsystemami. Trwałość i bezpieczeństwo przechowywania danych. Zachowanie uptime'u przy nieregularnych skokach obciążenia."/>
     <x v="4"/>
     <x v="2"/>
@@ -986,7 +2156,7 @@
   <r>
     <x v="10"/>
     <x v="3"/>
-    <x v="10"/>
+    <s v="Elastyczność kosztów"/>
     <s v="Możliwa jest różnica kosztów projektu wynikająca z nadgodzin, lub opóźnień, zidentyfikowanych w innych ryzykach."/>
     <x v="0"/>
     <x v="3"/>
@@ -995,7 +2165,7 @@
   <r>
     <x v="11"/>
     <x v="3"/>
-    <x v="11"/>
+    <s v="Elastyczność zakresu projektu"/>
     <s v="Ewentualne zmiany w zakresie projektu podyktowane żądaniami priorytetowych inwestorów."/>
     <x v="1"/>
     <x v="1"/>
@@ -1004,7 +2174,7 @@
   <r>
     <x v="12"/>
     <x v="3"/>
-    <x v="12"/>
+    <s v="Poparcie biznesowe inwestorów"/>
     <s v="Realizacja iteracji C &quot;Wdrożenie&quot; jest niemożliwa bez wczesnego wsparcia finansowego inwestorów."/>
     <x v="2"/>
     <x v="0"/>
@@ -1013,7 +2183,7 @@
   <r>
     <x v="13"/>
     <x v="3"/>
-    <x v="13"/>
+    <s v="Przyjęcie aplikacji mobilnej przez użytkowników"/>
     <m/>
     <x v="2"/>
     <x v="2"/>
@@ -1022,7 +2192,7 @@
   <r>
     <x v="14"/>
     <x v="4"/>
-    <x v="14"/>
+    <s v="Zbyt mała liczba współpracujących organizatorów"/>
     <s v="Zbyt mała ilość współpracujących organizatorów wydarzeń przełoży się na ubogą bazę materiałów referencyjnych w bazie. Dodatkowo, każdy współpracownik jest bezpośrednio związany z udzielanymi rabatami dla użytkowników. Zmniejszy to atrakcyjność oferty."/>
     <x v="2"/>
     <x v="4"/>
@@ -1031,7 +2201,7 @@
   <r>
     <x v="15"/>
     <x v="4"/>
-    <x v="15"/>
+    <s v="Jakość danych od partnerów"/>
     <s v="Niska jakość, bądź niekompletność danych dostarczanych przez współpracowników przełoży  się na nieefektywne, bądź błędne działanie naszego systemu. "/>
     <x v="4"/>
     <x v="4"/>
@@ -1040,7 +2210,7 @@
   <r>
     <x v="16"/>
     <x v="4"/>
-    <x v="16"/>
+    <s v="Usługi serwerowe"/>
     <s v="Dostawca usług serwerowych może nie zapewnić wystarczającej mocy obliczeniowej i skalowalności. Doprowadzi to do niskiej responsywności aplikacji, przekładającej się na satysfakcję użytkowania aplikacji mobilnej."/>
     <x v="3"/>
     <x v="0"/>
@@ -1049,7 +2219,7 @@
   <r>
     <x v="17"/>
     <x v="4"/>
-    <x v="17"/>
+    <s v="Konkurencja"/>
     <s v="Jeżeli inna firma zrealizuje podobny projekt przed nami, który stanie się bardzo popularny, to bardzo trudno będzie skłonić użytkowników do korzystania z nowopowstałej aplikacji."/>
     <x v="2"/>
     <x v="1"/>
@@ -1059,17 +2229,208 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba wystąpień" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria" colHeaderCaption="Wpływ">
+  <location ref="A1:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField axis="axisCol" numFmtId="1" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item n="Niski wpływ_x000a_(0-19)" x="1"/>
+        <item n="Średni wpływ_x000a_(20-39)" x="2"/>
+        <item n="Wysoki wpływ_x000a_(&gt; 40)" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="6"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Zliczenie ryzyk według wpływu" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="28">
+    <format dxfId="297">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="296">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="295">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="293">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="292">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="291">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="143">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="141">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="139">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="137">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="134">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="131">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="129">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="127">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="125">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="122">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="21">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="17">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="3">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="B1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight18" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba wystąpień" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A1:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField axis="axisRow" subtotalCaption="? - Suma" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
+        <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1096,39 +2457,113 @@
       </items>
     </pivotField>
     <pivotField compact="0" numFmtId="1" outline="0" showAll="0">
-      <items count="12">
+      <items count="5">
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="10"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="1"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="31">
     <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
       <x/>
     </i>
     <i>
       <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
     </i>
     <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
       <x v="2"/>
     </i>
     <i>
       <x v="3"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
     </i>
     <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
       <x v="4"/>
     </i>
     <i t="grand">
@@ -1158,71 +2593,52 @@
       <x/>
     </i>
   </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
-    <dataField name="Zliczenie ryzyk" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Zliczenie ryzyk według kosztów dla kategorii" fld="0" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
-  <formats count="12">
-    <format dxfId="11">
+  <formats count="8">
+    <format dxfId="313">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="314">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    <format dxfId="315">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="5" count="0"/>
-        </references>
-      </pivotArea>
+    <format dxfId="316">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="317">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4" count="0"/>
+          <reference field="5" count="1" selected="0">
+            <x v="4"/>
+          </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    <format dxfId="1">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="D1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="5" count="0"/>
+          <reference field="5" count="1">
+            <x v="4"/>
+          </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="5" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
   </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleMedium11" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -1555,26 +2971,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="8"/>
-    <col min="6" max="6" width="8.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="8"/>
-    <col min="8" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="8"/>
+    <col min="6" max="6" width="8.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="8"/>
+    <col min="8" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="28" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +3013,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="56">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>71</v>
       </c>
@@ -1608,7 +3024,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" s="10">
         <v>2</v>
@@ -1621,7 +3037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="56">
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>72</v>
       </c>
@@ -1629,10 +3045,10 @@
         <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -1645,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="84">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -1669,7 +3085,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="70">
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -1693,7 +3109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="56">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -1717,7 +3133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -1738,7 +3154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -1762,7 +3178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +3202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="56">
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -1810,7 +3226,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="56">
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
@@ -1834,7 +3250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="42">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -1858,7 +3274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="42">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -1882,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -1906,7 +3322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -1927,7 +3343,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="84">
+    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>81</v>
       </c>
@@ -1951,7 +3367,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="56">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
@@ -1975,7 +3391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="70">
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>83</v>
       </c>
@@ -1999,7 +3415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="56">
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>84</v>
       </c>
@@ -2035,13 +3451,6 @@
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
         <cfvo type="percent" val="50"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="2">
-      <iconSet>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>
@@ -2063,19 +3472,19 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="28" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -2089,7 +3498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>71</v>
       </c>
@@ -2104,7 +3513,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>72</v>
       </c>
@@ -2116,7 +3525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -2131,7 +3540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -2146,7 +3555,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -2161,7 +3570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -2173,7 +3582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -2188,7 +3597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -2203,7 +3612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="42">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -2218,7 +3627,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -2233,7 +3642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="42">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -2248,7 +3657,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -2263,7 +3672,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -2278,7 +3687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="42">
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -2293,7 +3702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -2308,7 +3717,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="42">
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
@@ -2323,7 +3732,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="42">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
@@ -2338,7 +3747,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>56</v>
       </c>
@@ -2353,7 +3762,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
@@ -2368,7 +3777,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28">
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>56</v>
       </c>
@@ -2383,7 +3792,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="42">
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>56</v>
       </c>
@@ -2398,7 +3807,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="42">
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>81</v>
       </c>
@@ -2413,7 +3822,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="70">
+    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>82</v>
       </c>
@@ -2428,7 +3837,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>82</v>
       </c>
@@ -2443,7 +3852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="56">
+    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>82</v>
       </c>
@@ -2458,7 +3867,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>83</v>
       </c>
@@ -2473,7 +3882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>84</v>
       </c>
@@ -2488,7 +3897,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="42">
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>84</v>
       </c>
@@ -2530,53 +3939,53 @@
       <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="8" width="20.83203125" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
+    <col min="3" max="8" width="20.85546875" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="22" customFormat="1" ht="28" customHeight="1">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" s="23" customFormat="1" ht="28" customHeight="1">
-      <c r="A2" s="26" t="s">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28">
+      <c r="G2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>71</v>
       </c>
@@ -2584,17 +3993,17 @@
         <f>VLOOKUP(A3, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Brak współpracy użytkowników w trakcie projektu</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="42">
+      <c r="C3" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -2602,17 +4011,17 @@
         <f>VLOOKUP(A4, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Zaangażowanie współpracujących organizatorów</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="42">
+      <c r="C4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
@@ -2620,11 +4029,11 @@
         <f>VLOOKUP(A5, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Niewystarczające kwalifikacje i doświadczenie członków zespołu</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28">
+      <c r="E5" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -2632,14 +4041,14 @@
         <f>VLOOKUP(A6, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Krytyczne uwarunkowania czasowe</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28" customHeight="1">
+      <c r="E6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -2647,11 +4056,11 @@
         <f>VLOOKUP(A7, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Gęstość pracochłonności</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28">
+      <c r="E7" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -2659,20 +4068,20 @@
         <f>VLOOKUP(A8, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Brak doświadczenia kierownika projektu</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28">
+      <c r="D8" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
@@ -2680,14 +4089,14 @@
         <f>VLOOKUP(A9, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Dynamiczność rynku technologii mobilnych</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28">
+      <c r="D9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>37</v>
       </c>
@@ -2695,14 +4104,14 @@
         <f>VLOOKUP(A10, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Jednoznaczność specyfikacji funkcjonalnej</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28" customHeight="1">
+      <c r="F10" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -2710,20 +4119,20 @@
         <f>VLOOKUP(A11, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Złożoność systemu</v>
       </c>
-      <c r="D11" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28" customHeight="1">
+      <c r="D11" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -2731,14 +4140,14 @@
         <f>VLOOKUP(A12, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Sprawność operacyjna</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28" customHeight="1">
+      <c r="C12" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -2746,14 +4155,14 @@
         <f>VLOOKUP(A13, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Elastyczność kosztów</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28" customHeight="1">
+      <c r="E13" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -2761,11 +4170,11 @@
         <f>VLOOKUP(A14, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Elastyczność zakresu projektu</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28" customHeight="1">
+      <c r="G14" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -2773,20 +4182,20 @@
         <f>VLOOKUP(A15, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Poparcie biznesowe inwestorów</v>
       </c>
-      <c r="D15" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28" customHeight="1">
+      <c r="D15" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
@@ -2794,14 +4203,14 @@
         <f>VLOOKUP(A16, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Przyjęcie aplikacji mobilnej przez użytkowników</v>
       </c>
-      <c r="D16" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="42" customHeight="1">
+      <c r="D16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>81</v>
       </c>
@@ -2809,11 +4218,11 @@
         <f>VLOOKUP(A17, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Zbyt mała liczba współpracujących organizatorów</v>
       </c>
-      <c r="G17" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="28" customHeight="1">
+      <c r="G17" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>82</v>
       </c>
@@ -2821,20 +4230,20 @@
         <f>VLOOKUP(A18, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Jakość danych od partnerów</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="28" customHeight="1">
+      <c r="C18" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -2842,20 +4251,20 @@
         <f>VLOOKUP(A19, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Usługi serwerowe</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28" customHeight="1">
+      <c r="C19" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>84</v>
       </c>
@@ -2863,8 +4272,8 @@
         <f>VLOOKUP(A20, Ryzyka!$A$1:$C$19, 3, FALSE)</f>
         <v>Konkurencja</v>
       </c>
-      <c r="G20" s="27" t="s">
-        <v>105</v>
+      <c r="G20" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2889,157 +4298,715 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.83203125" style="1"/>
+    <col min="1" max="1" width="23.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="12" width="3" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="20">
+        <v>2</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20">
+        <v>3</v>
+      </c>
+      <c r="D4" s="38">
+        <v>1</v>
+      </c>
+      <c r="E4" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="14">
-      <c r="A3" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="B5" s="20">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="38">
+        <v>1</v>
+      </c>
+      <c r="E5" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="20">
+        <v>2</v>
+      </c>
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="38">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="20">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="38">
+        <v>1</v>
+      </c>
+      <c r="E7" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="20">
+        <v>8</v>
+      </c>
+      <c r="C8" s="20">
+        <v>6</v>
+      </c>
+      <c r="D8" s="38">
+        <v>4</v>
+      </c>
+      <c r="E8" s="35">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="21" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20">
-        <v>1</v>
-      </c>
-      <c r="C4" s="20">
+      <c r="C2" s="26">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
         <v>2</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E2" s="26">
         <v>3</v>
       </c>
-      <c r="E4" s="20">
+      <c r="F2" s="26">
         <v>4</v>
       </c>
-      <c r="F4" s="20">
+      <c r="G2" s="40">
         <v>5</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H2" s="26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14">
-      <c r="A5" s="20">
-        <v>1</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" ht="14">
-      <c r="A6" s="20">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="29">
         <v>2</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="14">
-      <c r="A7" s="20">
+      <c r="C4" s="27"/>
+      <c r="D4" s="27">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="29">
         <v>4</v>
       </c>
-      <c r="B7" s="15">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="29">
+        <v>8</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="29">
+        <v>16</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="27">
+        <v>1</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="27">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14">
-      <c r="A8" s="20">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="29">
+        <v>2</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="29">
+        <v>4</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="41">
+        <v>1</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="29">
         <v>8</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" thickBot="1">
-      <c r="A9" s="20">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27">
+        <v>1</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="29">
         <v>16</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" thickTop="1">
-      <c r="A10" s="17" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27">
+        <v>1</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27">
+        <v>1</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27">
+        <v>2</v>
+      </c>
+      <c r="G14" s="41">
+        <v>1</v>
+      </c>
+      <c r="H14" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="29">
+        <v>2</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="29">
+        <v>4</v>
+      </c>
+      <c r="C17" s="27">
+        <v>1</v>
+      </c>
+      <c r="D17" s="27">
+        <v>1</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="29">
+        <v>8</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27">
+        <v>1</v>
+      </c>
+      <c r="G18" s="41"/>
+      <c r="H18" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="29">
+        <v>16</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="41">
+        <v>1</v>
+      </c>
+      <c r="H19" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="27">
+        <v>1</v>
+      </c>
+      <c r="D20" s="27">
+        <v>1</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27">
+        <v>1</v>
+      </c>
+      <c r="G20" s="41">
+        <v>1</v>
+      </c>
+      <c r="H20" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="29">
+        <v>1</v>
+      </c>
+      <c r="C21" s="27">
+        <v>1</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25"/>
+      <c r="B22" s="29">
+        <v>2</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="41">
+        <v>1</v>
+      </c>
+      <c r="H22" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
+      <c r="B23" s="29">
+        <v>4</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="29">
+        <v>8</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="29">
+        <v>16</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27">
+        <v>1</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27">
+        <v>1</v>
+      </c>
+      <c r="G25" s="41"/>
+      <c r="H25" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="27">
+        <v>1</v>
+      </c>
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27">
+        <v>1</v>
+      </c>
+      <c r="G26" s="41">
+        <v>1</v>
+      </c>
+      <c r="H26" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="29">
+        <v>2</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="29">
+        <v>4</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27">
+        <v>1</v>
+      </c>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="29">
+        <v>8</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27">
+        <v>1</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="29">
+        <v>16</v>
+      </c>
+      <c r="C31" s="27">
+        <v>1</v>
+      </c>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27">
+        <v>1</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="27">
+        <v>1</v>
+      </c>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="27">
+        <v>2</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-      <c r="C10" s="18">
-        <v>1</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="B33" s="25"/>
+      <c r="C33" s="27">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" ht="15" customHeight="1">
-      <c r="C18" s="1" t="s">
-        <v>97</v>
+      <c r="D33" s="27">
+        <v>5</v>
+      </c>
+      <c r="E33" s="27">
+        <v>2</v>
+      </c>
+      <c r="F33" s="27">
+        <v>4</v>
+      </c>
+      <c r="G33" s="41">
+        <v>3</v>
+      </c>
+      <c r="H33" s="27">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Popraw formatowanie tabel zbiorczych
</commit_message>
<xml_diff>
--- a/Cwiczenie-4/Ryzyka.xlsx
+++ b/Cwiczenie-4/Ryzyka.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="16440" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="16440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzyka" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="26" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="117">
   <si>
     <t>Zmniejszenie wpływu</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>Przy braku funduszy w bardzo wczesnej fazie projektu, znalezienie środków w kredycie, funduszach EU lub mafii.</t>
-  </si>
-  <si>
-    <t>Liczba wystąpień</t>
   </si>
   <si>
     <t>Nawiązanie współpracy z organizatorami</t>
@@ -367,9 +364,6 @@
     <t>Nie zrozumienie funkcjonalności aplikacji mobilnej. Niska intucyjność obsługi, niska ocena wyglądu aplikacji. Błędna analiza wymagań użytkowników aplikacji.</t>
   </si>
   <si>
-    <t>Zliczenie ryzyk według kosztów dla kategorii</t>
-  </si>
-  <si>
     <t>Organizacyjne - Suma</t>
   </si>
   <si>
@@ -401,6 +395,9 @@
   <si>
     <t>Wysoki wpływ
 (&gt; 40)</t>
+  </si>
+  <si>
+    <t>Zliczenie ryzyk według kosztów i prawdopod. dla kategorii</t>
   </si>
 </sst>
 </file>
@@ -650,12 +647,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -714,6 +705,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Excel Built-in Normal" xfId="9"/>
@@ -769,34 +766,766 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="318">
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </right>
-      </border>
+  <dxfs count="180">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -808,21 +1537,7 @@
     <dxf>
       <border>
         <right style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
           <color theme="6" tint="0.39997558519241921"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="0.59999389629810485"/>
         </right>
       </border>
     </dxf>
@@ -855,55 +1570,52 @@
       </border>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -929,1023 +1641,6 @@
       <font>
         <b/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2229,7 +1924,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria" colHeaderCaption="Wpływ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria" colHeaderCaption="Wpływ">
   <location ref="A1:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -2301,71 +1996,71 @@
     <dataField name="Zliczenie ryzyk według wpływu" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="297">
+    <format dxfId="179">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="296">
+    <format dxfId="178">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="295">
+    <format dxfId="177">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="293">
+    <format dxfId="176">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="292">
+    <format dxfId="175">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="291">
+    <format dxfId="174">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="143">
+    <format dxfId="173">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="141">
+    <format dxfId="172">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="139">
+    <format dxfId="171">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="137">
+    <format dxfId="170">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="134">
+    <format dxfId="169">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="131">
+    <format dxfId="168">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="129">
+    <format dxfId="167">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="127">
+    <format dxfId="166">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="125">
+    <format dxfId="165">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="164">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="163">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="162">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="161">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="160">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="159">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="3">
@@ -2376,19 +2071,19 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="158">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="157">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="156">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="155">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="154">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" selected="0">
@@ -2397,10 +2092,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="153">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="B1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="152">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2410,7 +2105,7 @@
       </pivotArea>
     </format>
   </formats>
-  <pivotTableStyleInfo name="PivotStyleLight18" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleMedium11" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -2420,7 +2115,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba wystąpień" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -2594,29 +2289,29 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Zliczenie ryzyk według kosztów dla kategorii" fld="0" subtotal="count" baseField="4" baseItem="0"/>
+    <dataField name="Zliczenie ryzyk według kosztów i prawdopod. dla kategorii" fld="0" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="313">
+    <format dxfId="151">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="314">
+    <format dxfId="150">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="315">
+    <format dxfId="149">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="316">
+    <format dxfId="148">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="317">
+    <format dxfId="147">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="146">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1" selected="0">
@@ -2625,10 +2320,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="145">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="D1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="144">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2972,25 +2667,25 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="8"/>
-    <col min="6" max="6" width="8.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8"/>
-    <col min="8" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="8"/>
+    <col min="6" max="6" width="8.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="8"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -3013,7 +2708,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="56">
       <c r="A2" s="12" t="s">
         <v>71</v>
       </c>
@@ -3024,7 +2719,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E2" s="10">
         <v>2</v>
@@ -3037,7 +2732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="56">
       <c r="A3" s="12" t="s">
         <v>72</v>
       </c>
@@ -3045,10 +2740,10 @@
         <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -3061,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="84">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -3085,7 +2780,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="70">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -3109,7 +2804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="56">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -3133,7 +2828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -3154,7 +2849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="42">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -3178,7 +2873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -3202,7 +2897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="56">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -3226,7 +2921,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="56">
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
@@ -3250,7 +2945,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="42">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -3274,7 +2969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="42">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -3298,7 +2993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -3322,7 +3017,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -3343,7 +3038,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="84">
       <c r="A16" s="12" t="s">
         <v>81</v>
       </c>
@@ -3367,7 +3062,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="56">
       <c r="A17" s="12" t="s">
         <v>82</v>
       </c>
@@ -3391,7 +3086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="70">
       <c r="A18" s="12" t="s">
         <v>83</v>
       </c>
@@ -3415,7 +3110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="56">
       <c r="A19" s="12" t="s">
         <v>84</v>
       </c>
@@ -3475,16 +3170,16 @@
       <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3498,7 +3193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28">
       <c r="A2" s="12" t="s">
         <v>71</v>
       </c>
@@ -3513,7 +3208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="42">
       <c r="A3" s="12" t="s">
         <v>72</v>
       </c>
@@ -3525,7 +3220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="42">
       <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
@@ -3540,7 +3235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -3555,7 +3250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
@@ -3570,7 +3265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
@@ -3582,7 +3277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
@@ -3597,7 +3292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="12" t="s">
         <v>37</v>
       </c>
@@ -3612,7 +3307,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="42">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -3627,7 +3322,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -3642,7 +3337,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="42">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -3657,7 +3352,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -3672,7 +3367,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -3687,7 +3382,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="42">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -3702,7 +3397,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28">
       <c r="A16" s="12" t="s">
         <v>55</v>
       </c>
@@ -3717,7 +3412,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="42">
       <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
@@ -3732,7 +3427,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="42">
       <c r="A18" s="12" t="s">
         <v>55</v>
       </c>
@@ -3747,7 +3442,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28">
       <c r="A19" s="12" t="s">
         <v>56</v>
       </c>
@@ -3762,7 +3457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28">
       <c r="A20" s="12" t="s">
         <v>56</v>
       </c>
@@ -3777,7 +3472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28">
       <c r="A21" s="12" t="s">
         <v>56</v>
       </c>
@@ -3792,7 +3487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="42">
       <c r="A22" s="12" t="s">
         <v>56</v>
       </c>
@@ -3807,7 +3502,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="42">
       <c r="A23" s="12" t="s">
         <v>81</v>
       </c>
@@ -3822,7 +3517,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="70">
       <c r="A24" s="12" t="s">
         <v>82</v>
       </c>
@@ -3837,7 +3532,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28">
       <c r="A25" s="12" t="s">
         <v>82</v>
       </c>
@@ -3852,7 +3547,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="56">
       <c r="A26" s="12" t="s">
         <v>82</v>
       </c>
@@ -3867,7 +3562,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="28">
       <c r="A27" s="12" t="s">
         <v>83</v>
       </c>
@@ -3882,7 +3577,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
         <v>84</v>
       </c>
@@ -3897,7 +3592,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="42">
       <c r="A29" s="12" t="s">
         <v>84</v>
       </c>
@@ -3939,27 +3634,27 @@
       <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="8" width="20.85546875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="8" width="20.83203125" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-    </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="13" customFormat="1" ht="28" customHeight="1">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+    </row>
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="28" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
@@ -3967,25 +3662,25 @@
         <v>88</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>101</v>
-      </c>
       <c r="G2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="28">
       <c r="A3" s="12" t="s">
         <v>71</v>
       </c>
@@ -3994,16 +3689,16 @@
         <v>Brak współpracy użytkowników w trakcie projektu</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="42">
       <c r="A4" s="12" t="s">
         <v>72</v>
       </c>
@@ -4012,16 +3707,16 @@
         <v>Zaangażowanie współpracujących organizatorów</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42">
       <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
@@ -4030,10 +3725,10 @@
         <v>Niewystarczające kwalifikacje i doświadczenie członków zespołu</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -4042,13 +3737,13 @@
         <v>Krytyczne uwarunkowania czasowe</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
@@ -4057,10 +3752,10 @@
         <v>Gęstość pracochłonności</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28">
       <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
@@ -4069,19 +3764,19 @@
         <v>Brak doświadczenia kierownika projektu</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28">
       <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
@@ -4090,13 +3785,13 @@
         <v>Dynamiczność rynku technologii mobilnych</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28">
       <c r="A10" s="12" t="s">
         <v>37</v>
       </c>
@@ -4105,13 +3800,13 @@
         <v>Jednoznaczność specyfikacji funkcjonalnej</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -4120,19 +3815,19 @@
         <v>Złożoność systemu</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
@@ -4141,13 +3836,13 @@
         <v>Sprawność operacyjna</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -4156,13 +3851,13 @@
         <v>Elastyczność kosztów</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -4171,10 +3866,10 @@
         <v>Elastyczność zakresu projektu</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -4183,19 +3878,19 @@
         <v>Poparcie biznesowe inwestorów</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
@@ -4204,13 +3899,13 @@
         <v>Przyjęcie aplikacji mobilnej przez użytkowników</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>81</v>
       </c>
@@ -4219,10 +3914,10 @@
         <v>Zbyt mała liczba współpracujących organizatorów</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>82</v>
       </c>
@@ -4231,19 +3926,19 @@
         <v>Jakość danych od partnerów</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28" customHeight="1">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -4252,19 +3947,19 @@
         <v>Usługi serwerowe</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28" customHeight="1">
       <c r="A20" s="12" t="s">
         <v>84</v>
       </c>
@@ -4273,7 +3968,7 @@
         <v>Konkurencja</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -4300,149 +3995,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="20" customWidth="1"/>
+    <col min="6" max="14" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:5" ht="28">
+      <c r="A1" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="28">
+      <c r="A2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="E2" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="35">
+      <c r="C3" s="18"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18">
         <v>3</v>
       </c>
-      <c r="D4" s="38">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35">
+      <c r="D4" s="36">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="20">
-        <v>1</v>
-      </c>
-      <c r="D5" s="38">
-        <v>1</v>
-      </c>
-      <c r="E5" s="35">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="36">
+        <v>1</v>
+      </c>
+      <c r="E5" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C6" s="20">
-        <v>1</v>
-      </c>
-      <c r="D6" s="38">
-        <v>1</v>
-      </c>
-      <c r="E6" s="35">
+      <c r="C6" s="18">
+        <v>1</v>
+      </c>
+      <c r="D6" s="36">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="18">
         <v>2</v>
       </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="38">
-        <v>1</v>
-      </c>
-      <c r="E7" s="35">
+      <c r="C7" s="18">
+        <v>1</v>
+      </c>
+      <c r="D7" s="36">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="20">
+    <row r="8" spans="1:5">
+      <c r="A8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="18">
         <v>8</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <v>6</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="36">
         <v>4</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="33">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4450,563 +4145,560 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="12.85546875" style="1"/>
+    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
+    <col min="2" max="8" width="12.83203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8" ht="28">
+      <c r="A1" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" ht="14">
+      <c r="A2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="24">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24">
+        <v>2</v>
+      </c>
+      <c r="E2" s="24">
+        <v>3</v>
+      </c>
+      <c r="F2" s="24">
+        <v>4</v>
+      </c>
+      <c r="G2" s="38">
+        <v>5</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14">
+      <c r="A3" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14">
+      <c r="A4" s="23"/>
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14">
+      <c r="A5" s="23"/>
+      <c r="B5" s="27">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" ht="14">
+      <c r="A6" s="23"/>
+      <c r="B6" s="27">
+        <v>8</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" ht="14">
+      <c r="A7" s="23"/>
+      <c r="B7" s="27">
+        <v>16</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" ht="14">
+      <c r="A8" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="25">
+        <v>1</v>
+      </c>
+      <c r="D8" s="25">
+        <v>1</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14">
+      <c r="A9" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="27">
+        <v>1</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="1:8" ht="14">
+      <c r="A10" s="23"/>
+      <c r="B10" s="27">
+        <v>2</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" ht="14">
+      <c r="A11" s="23"/>
+      <c r="B11" s="27">
+        <v>4</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="39">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14">
+      <c r="A12" s="23"/>
+      <c r="B12" s="27">
+        <v>8</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14">
+      <c r="A13" s="23"/>
+      <c r="B13" s="27">
+        <v>16</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25">
+        <v>1</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="A14" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="26">
-        <v>1</v>
-      </c>
-      <c r="D2" s="26">
+      <c r="B14" s="23"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25">
         <v>2</v>
       </c>
-      <c r="E2" s="26">
+      <c r="G14" s="39">
+        <v>1</v>
+      </c>
+      <c r="H14" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14">
+      <c r="A15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="27">
+        <v>1</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:8" ht="14">
+      <c r="A16" s="23"/>
+      <c r="B16" s="27">
+        <v>2</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="1:8" ht="14">
+      <c r="A17" s="23"/>
+      <c r="B17" s="27">
+        <v>4</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25">
+        <v>1</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14">
+      <c r="A18" s="23"/>
+      <c r="B18" s="27">
+        <v>8</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25">
+        <v>1</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14">
+      <c r="A19" s="23"/>
+      <c r="B19" s="27">
+        <v>16</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="39">
+        <v>1</v>
+      </c>
+      <c r="H19" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="A20" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="25">
+        <v>1</v>
+      </c>
+      <c r="D20" s="25">
+        <v>1</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25">
+        <v>1</v>
+      </c>
+      <c r="G20" s="39">
+        <v>1</v>
+      </c>
+      <c r="H20" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14">
+      <c r="A21" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14">
+      <c r="A22" s="23"/>
+      <c r="B22" s="27">
+        <v>2</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="39">
+        <v>1</v>
+      </c>
+      <c r="H22" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14">
+      <c r="A23" s="23"/>
+      <c r="B23" s="27">
+        <v>4</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" ht="14">
+      <c r="A24" s="23"/>
+      <c r="B24" s="27">
+        <v>8</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" ht="14">
+      <c r="A25" s="23"/>
+      <c r="B25" s="27">
+        <v>16</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="39"/>
+      <c r="H25" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="A26" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="25">
+        <v>1</v>
+      </c>
+      <c r="D26" s="25">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25">
+        <v>1</v>
+      </c>
+      <c r="G26" s="39">
+        <v>1</v>
+      </c>
+      <c r="H26" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14">
+      <c r="A27" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" ht="14">
+      <c r="A28" s="23"/>
+      <c r="B28" s="27">
+        <v>2</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="14">
+      <c r="A29" s="23"/>
+      <c r="B29" s="27">
+        <v>4</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25">
+        <v>1</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14">
+      <c r="A30" s="23"/>
+      <c r="B30" s="27">
+        <v>8</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25">
+        <v>1</v>
+      </c>
+      <c r="F30" s="25"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="14">
+      <c r="A31" s="23"/>
+      <c r="B31" s="27">
+        <v>16</v>
+      </c>
+      <c r="C31" s="25">
+        <v>1</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25">
+        <v>1</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1">
+      <c r="A32" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="25">
+        <v>1</v>
+      </c>
+      <c r="D32" s="25">
+        <v>1</v>
+      </c>
+      <c r="E32" s="25">
+        <v>2</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1">
+      <c r="A33" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="25">
+        <v>4</v>
+      </c>
+      <c r="D33" s="25">
+        <v>5</v>
+      </c>
+      <c r="E33" s="25">
+        <v>2</v>
+      </c>
+      <c r="F33" s="25">
+        <v>4</v>
+      </c>
+      <c r="G33" s="39">
         <v>3</v>
       </c>
-      <c r="F2" s="26">
-        <v>4</v>
-      </c>
-      <c r="G2" s="40">
-        <v>5</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="29">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="29">
-        <v>2</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27">
-        <v>1</v>
-      </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="29">
-        <v>4</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="27"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="29">
-        <v>8</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="27"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="29">
-        <v>16</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="27"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="27">
-        <v>1</v>
-      </c>
-      <c r="D8" s="27">
-        <v>1</v>
-      </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="29">
-        <v>1</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="27"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="29">
-        <v>2</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="29">
-        <v>4</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="41">
-        <v>1</v>
-      </c>
-      <c r="H11" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="29">
-        <v>8</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27">
-        <v>1</v>
-      </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="29">
-        <v>16</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27">
-        <v>1</v>
-      </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27">
-        <v>1</v>
-      </c>
-      <c r="G13" s="41"/>
-      <c r="H13" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27">
-        <v>1</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27">
-        <v>2</v>
-      </c>
-      <c r="G14" s="41">
-        <v>1</v>
-      </c>
-      <c r="H14" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="29">
-        <v>1</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="29">
-        <v>2</v>
-      </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="27"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="29">
-        <v>4</v>
-      </c>
-      <c r="C17" s="27">
-        <v>1</v>
-      </c>
-      <c r="D17" s="27">
-        <v>1</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="29">
-        <v>8</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27">
-        <v>1</v>
-      </c>
-      <c r="G18" s="41"/>
-      <c r="H18" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="29">
-        <v>16</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="41">
-        <v>1</v>
-      </c>
-      <c r="H19" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="27">
-        <v>1</v>
-      </c>
-      <c r="D20" s="27">
-        <v>1</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27">
-        <v>1</v>
-      </c>
-      <c r="G20" s="41">
-        <v>1</v>
-      </c>
-      <c r="H20" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="29">
-        <v>1</v>
-      </c>
-      <c r="C21" s="27">
-        <v>1</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="29">
-        <v>2</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="41">
-        <v>1</v>
-      </c>
-      <c r="H22" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="29">
-        <v>4</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="29">
-        <v>8</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="29">
-        <v>16</v>
-      </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27">
-        <v>1</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27">
-        <v>1</v>
-      </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="27">
-        <v>1</v>
-      </c>
-      <c r="D26" s="27">
-        <v>1</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27">
-        <v>1</v>
-      </c>
-      <c r="G26" s="41">
-        <v>1</v>
-      </c>
-      <c r="H26" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="29">
-        <v>1</v>
-      </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="29">
-        <v>2</v>
-      </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="29">
-        <v>4</v>
-      </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27">
-        <v>1</v>
-      </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="29">
-        <v>8</v>
-      </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27">
-        <v>1</v>
-      </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="29">
-        <v>16</v>
-      </c>
-      <c r="C31" s="27">
-        <v>1</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27">
-        <v>1</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="27">
-        <v>1</v>
-      </c>
-      <c r="D32" s="27">
-        <v>1</v>
-      </c>
-      <c r="E32" s="27">
-        <v>2</v>
-      </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="27">
-        <v>4</v>
-      </c>
-      <c r="D33" s="27">
-        <v>5</v>
-      </c>
-      <c r="E33" s="27">
-        <v>2</v>
-      </c>
-      <c r="F33" s="27">
-        <v>4</v>
-      </c>
-      <c r="G33" s="41">
-        <v>3</v>
-      </c>
-      <c r="H33" s="27">
+      <c r="H33" s="25">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Dodaj parę wykresów do ryzyk
</commit_message>
<xml_diff>
--- a/Cwiczenie-4/Ryzyka.xlsx
+++ b/Cwiczenie-4/Ryzyka.xlsx
@@ -2,25 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
-  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="16440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28500" windowHeight="21080" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzyka" sheetId="1" r:id="rId1"/>
     <sheet name="Mitygacja" sheetId="4" r:id="rId2"/>
     <sheet name="Powiązanie z celami" sheetId="9" r:id="rId3"/>
-    <sheet name="Zliczenie ryzyk" sheetId="17" r:id="rId4"/>
-    <sheet name="Zliczenie ryzyk szczegółowe" sheetId="6" r:id="rId5"/>
+    <sheet name="Suma wpływu ryzyk" sheetId="18" r:id="rId4"/>
+    <sheet name="Zliczenie ryzyk" sheetId="17" r:id="rId5"/>
+    <sheet name="Zliczenie ryzyk szczegółowe" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mitygacja!$A$1:$D$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Powiązanie z celami'!$A$2:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ryzyka!$A$1:$G$19</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="119">
   <si>
     <t>Zmniejszenie wpływu</t>
   </si>
@@ -398,6 +399,12 @@
   </si>
   <si>
     <t>Zliczenie ryzyk według kosztów i prawdopod. dla kategorii</t>
+  </si>
+  <si>
+    <t>Suma wpływu ryzyk</t>
+  </si>
+  <si>
+    <t>Podsumowanie według kategorii</t>
   </si>
 </sst>
 </file>
@@ -524,17 +531,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
+        <color theme="6" tint="-0.249977111117893"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color theme="6" tint="-0.249977111117893"/>
-      </right>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -594,7 +601,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -685,24 +692,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -710,6 +706,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -766,725 +780,47 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="180">
+  <dxfs count="43">
     <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
+      <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
+      <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
+      <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+      <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
-        <right style="thin">
+        <left style="thin">
           <color theme="6" tint="-0.249977111117893"/>
-        </right>
+        </left>
       </border>
     </dxf>
     <dxf>
       <border>
-        <right style="thin">
+        <left style="thin">
           <color theme="6" tint="-0.249977111117893"/>
-        </right>
+        </left>
       </border>
     </dxf>
     <dxf>
       <border>
-        <right style="thin">
+        <left style="thin">
           <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
+        </left>
       </border>
     </dxf>
     <dxf>
@@ -1546,27 +882,6 @@
         <right style="thin">
           <color theme="6" tint="0.39997558519241921"/>
         </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF92D050"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF92D050"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF92D050"/>
-        </left>
       </border>
     </dxf>
     <dxf>
@@ -1651,6 +966,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFDC3E20"/>
+      <color rgb="FFFFDF1F"/>
+      <color rgb="FF92D050"/>
       <color rgb="FFCCFF99"/>
     </mruColors>
   </colors>
@@ -1660,6 +978,542 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="137"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="37"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Suma wpływu ryzyk</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Suma wpływu ryzyk'!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Organizacyjne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Zewnętrznych zależności</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Założeń opłacalności</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Techniczne</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Planowanie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Suma wpływu ryzyk'!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>148.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2132643832"/>
+        <c:axId val="2132049192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2132643832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132049192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2132049192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2132643832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="134"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="34"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wysoki wpływ_x000d_(&gt; 40)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3E20"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Organizacyjne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planowanie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Techniczne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Założeń opłacalności</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Zewnętrznych zależności</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zliczenie ryzyk'!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Średni wpływ_x000d_(20-39)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFDF1F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Organizacyjne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planowanie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Techniczne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Założeń opłacalności</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Zewnętrznych zależności</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zliczenie ryzyk'!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Niski wpływ_x000d_(0-19)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Zliczenie ryzyk'!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Organizacyjne</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planowanie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Techniczne</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Założeń opłacalności</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Zewnętrznych zależności</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Zliczenie ryzyk'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2074526232"/>
+        <c:axId val="2076703256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2074526232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2076703256"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2076703256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> ryzyk</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2074526232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2116</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1924,7 +1778,99 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria" colHeaderCaption="Wpływ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Podsumowanie według kategorii" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria">
+  <location ref="A1:C7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField dataField="1" showAll="0">
+      <items count="19">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Liczba ryzyk" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Suma wpływu ryzyk" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="6">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium11" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Kategoria" colHeaderCaption="Wpływ">
   <location ref="A1:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -1996,71 +1942,71 @@
     <dataField name="Zliczenie ryzyk według wpływu" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="179">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="178">
+    <format dxfId="41">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="177">
+    <format dxfId="40">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="176">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="175">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="174">
+    <format dxfId="37">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="173">
+    <format dxfId="36">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="172">
+    <format dxfId="35">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="171">
+    <format dxfId="34">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="170">
+    <format dxfId="33">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="169">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="168">
+    <format dxfId="31">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="167">
+    <format dxfId="30">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="166">
+    <format dxfId="29">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="165">
+    <format dxfId="28">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="164">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="163">
+    <format dxfId="26">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="162">
+    <format dxfId="25">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="161">
+    <format dxfId="24">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="160">
+    <format dxfId="23">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="159">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="3">
@@ -2071,19 +2017,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="158">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="157">
-      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="156">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1" fieldPosition="0"/>
-    </format>
-    <format dxfId="155">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="154">
+    <format dxfId="20">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1" selected="0">
@@ -2092,10 +2029,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="153">
+    <format dxfId="19">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="B1" fieldPosition="0"/>
     </format>
-    <format dxfId="152">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="1">
@@ -2103,6 +2040,15 @@
           </reference>
         </references>
       </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1" fieldPosition="0"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium11" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -2114,8 +2060,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Liczba ryzyk" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:H33" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -2292,26 +2238,26 @@
     <dataField name="Zliczenie ryzyk według kosztów i prawdopod. dla kategorii" fld="0" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="151">
+    <format dxfId="17">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="150">
+    <format dxfId="16">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="149">
+    <format dxfId="15">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="148">
+    <format dxfId="14">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="147">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="146">
+    <format dxfId="12">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1" selected="0">
@@ -2320,10 +2266,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="145">
+    <format dxfId="11">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="D1" fieldPosition="0"/>
     </format>
-    <format dxfId="144">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2667,10 +2613,10 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" sqref="A1:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3643,16 +3589,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="13" customFormat="1" ht="28" customHeight="1">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="40" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" s="14" customFormat="1" ht="28" customHeight="1">
       <c r="A2" s="15" t="s">
@@ -3993,9 +3939,110 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28">
+      <c r="B1" s="44" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="18">
+        <v>2</v>
+      </c>
+      <c r="C3" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="18">
+        <v>4</v>
+      </c>
+      <c r="C4" s="18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="18">
+        <v>4</v>
+      </c>
+      <c r="C5" s="18">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="18">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>4</v>
+      </c>
+      <c r="C7" s="18">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C7">
+    <sortCondition ref="C3"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -4015,8 +4062,8 @@
         <v>59</v>
       </c>
       <c r="C1" s="28"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" s="20" customFormat="1" ht="28">
       <c r="A2" s="30" t="s">
@@ -4028,10 +4075,10 @@
       <c r="C2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="40" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4043,8 +4090,8 @@
         <v>2</v>
       </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="33">
+      <c r="D3" s="38"/>
+      <c r="E3" s="41">
         <v>2</v>
       </c>
     </row>
@@ -4056,10 +4103,10 @@
       <c r="C4" s="18">
         <v>3</v>
       </c>
-      <c r="D4" s="36">
-        <v>1</v>
-      </c>
-      <c r="E4" s="33">
+      <c r="D4" s="38">
+        <v>1</v>
+      </c>
+      <c r="E4" s="41">
         <v>4</v>
       </c>
     </row>
@@ -4073,10 +4120,10 @@
       <c r="C5" s="18">
         <v>1</v>
       </c>
-      <c r="D5" s="36">
-        <v>1</v>
-      </c>
-      <c r="E5" s="33">
+      <c r="D5" s="38">
+        <v>1</v>
+      </c>
+      <c r="E5" s="41">
         <v>4</v>
       </c>
     </row>
@@ -4090,10 +4137,10 @@
       <c r="C6" s="18">
         <v>1</v>
       </c>
-      <c r="D6" s="36">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33">
+      <c r="D6" s="38">
+        <v>1</v>
+      </c>
+      <c r="E6" s="41">
         <v>4</v>
       </c>
     </row>
@@ -4107,10 +4154,10 @@
       <c r="C7" s="18">
         <v>1</v>
       </c>
-      <c r="D7" s="36">
-        <v>1</v>
-      </c>
-      <c r="E7" s="33">
+      <c r="D7" s="38">
+        <v>1</v>
+      </c>
+      <c r="E7" s="41">
         <v>4</v>
       </c>
     </row>
@@ -4124,15 +4171,16 @@
       <c r="C8" s="18">
         <v>6</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="38">
         <v>4</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="41">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4141,11 +4189,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -4167,7 +4215,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
-      <c r="G1" s="37"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="14">
@@ -4189,7 +4237,7 @@
       <c r="F2" s="24">
         <v>4</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="33">
         <v>5</v>
       </c>
       <c r="H2" s="24" t="s">
@@ -4209,7 +4257,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
-      <c r="G3" s="39"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="25">
         <v>1</v>
       </c>
@@ -4225,7 +4273,7 @@
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="39"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="25">
         <v>1</v>
       </c>
@@ -4239,7 +4287,7 @@
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
-      <c r="G5" s="39"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="14">
@@ -4251,7 +4299,7 @@
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="14">
@@ -4263,7 +4311,7 @@
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="39"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" ht="14">
@@ -4279,7 +4327,7 @@
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
-      <c r="G8" s="39"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="25">
         <v>2</v>
       </c>
@@ -4295,7 +4343,7 @@
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="39"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" ht="14">
@@ -4307,7 +4355,7 @@
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="39"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" ht="14">
@@ -4319,7 +4367,7 @@
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="39">
+      <c r="G11" s="34">
         <v>1</v>
       </c>
       <c r="H11" s="25">
@@ -4337,7 +4385,7 @@
       <c r="F12" s="25">
         <v>1</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="25">
         <v>1</v>
       </c>
@@ -4355,7 +4403,7 @@
       <c r="F13" s="25">
         <v>1</v>
       </c>
-      <c r="G13" s="39"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="25">
         <v>2</v>
       </c>
@@ -4373,7 +4421,7 @@
       <c r="F14" s="25">
         <v>2</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="34">
         <v>1</v>
       </c>
       <c r="H14" s="25">
@@ -4391,7 +4439,7 @@
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="39"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="14">
@@ -4403,7 +4451,7 @@
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
-      <c r="G16" s="39"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" ht="14">
@@ -4419,7 +4467,7 @@
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
-      <c r="G17" s="39"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="25">
         <v>2</v>
       </c>
@@ -4435,7 +4483,7 @@
       <c r="F18" s="25">
         <v>1</v>
       </c>
-      <c r="G18" s="39"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="25">
         <v>1</v>
       </c>
@@ -4449,7 +4497,7 @@
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="39">
+      <c r="G19" s="34">
         <v>1</v>
       </c>
       <c r="H19" s="25">
@@ -4471,7 +4519,7 @@
       <c r="F20" s="25">
         <v>1</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="34">
         <v>1</v>
       </c>
       <c r="H20" s="25">
@@ -4491,7 +4539,7 @@
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
-      <c r="G21" s="39"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="25">
         <v>1</v>
       </c>
@@ -4505,7 +4553,7 @@
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="39">
+      <c r="G22" s="34">
         <v>1</v>
       </c>
       <c r="H22" s="25">
@@ -4521,7 +4569,7 @@
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="39"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" ht="14">
@@ -4533,7 +4581,7 @@
       <c r="D24" s="25"/>
       <c r="E24" s="25"/>
       <c r="F24" s="25"/>
-      <c r="G24" s="39"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" ht="14">
@@ -4549,7 +4597,7 @@
       <c r="F25" s="25">
         <v>1</v>
       </c>
-      <c r="G25" s="39"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="25">
         <v>2</v>
       </c>
@@ -4569,7 +4617,7 @@
       <c r="F26" s="25">
         <v>1</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="34">
         <v>1</v>
       </c>
       <c r="H26" s="25">
@@ -4587,7 +4635,7 @@
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
-      <c r="G27" s="39"/>
+      <c r="G27" s="34"/>
       <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:8" ht="14">
@@ -4599,7 +4647,7 @@
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
-      <c r="G28" s="39"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="25"/>
     </row>
     <row r="29" spans="1:8" ht="14">
@@ -4613,7 +4661,7 @@
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="39"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="25">
         <v>1</v>
       </c>
@@ -4629,7 +4677,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="25"/>
-      <c r="G30" s="39"/>
+      <c r="G30" s="34"/>
       <c r="H30" s="25">
         <v>1</v>
       </c>
@@ -4647,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="25"/>
-      <c r="G31" s="39"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="25">
         <v>2</v>
       </c>
@@ -4667,7 +4715,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="25"/>
-      <c r="G32" s="39"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="25">
         <v>4</v>
       </c>
@@ -4689,7 +4737,7 @@
       <c r="F33" s="25">
         <v>4</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="34">
         <v>3</v>
       </c>
       <c r="H33" s="25">

</xml_diff>